<commit_message>
update schema 1.5: eaf not mandatory
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.5.xlsx
+++ b/schema_definitions/template_schema_v1.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC3C0FA-46A2-8B40-BB8E-C0136F40576E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1CB454-9877-3249-B396-21617B92B43E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30860" yWindow="-4160" windowWidth="46620" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1730,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Added changes to cater for curator-driven templates and GCST lists.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.5.xlsx
+++ b/schema_definitions/template_schema_v1.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/gwas-template-services/schema_definitions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Desktop/__FUNNY__/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1CB454-9877-3249-B396-21617B92B43E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DBB7ED-4C03-0E4E-97C2-05BECA83FC89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="36860" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="183">
   <si>
     <t>NAME</t>
   </si>
@@ -581,6 +581,12 @@
   </si>
   <si>
     <t>Genome assembly for the summary statistics. 'NR' if not providing summary statistics.</t>
+  </si>
+  <si>
+    <t>MANDATORY-CURATOR</t>
+  </si>
+  <si>
+    <t>MANDATORY-GCST</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,17 +1017,18 @@
     <col min="3" max="3" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="5"/>
-    <col min="9" max="9" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="5"/>
-    <col min="12" max="12" width="23.6640625" style="5" customWidth="1"/>
-    <col min="13" max="14" width="44.5" style="7" customWidth="1"/>
-    <col min="15" max="15" width="96" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="5"/>
+    <col min="6" max="7" width="22" style="5" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="5"/>
+    <col min="11" max="11" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="5"/>
+    <col min="14" max="14" width="23.6640625" style="5" customWidth="1"/>
+    <col min="15" max="16" width="44.5" style="7" customWidth="1"/>
+    <col min="17" max="17" width="96" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1038,37 +1045,43 @@
         <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1087,17 +1100,23 @@
       <c r="F2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O2" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>143</v>
       </c>
@@ -1116,23 +1135,29 @@
       <c r="F3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="M3" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1149,26 +1174,32 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="L4" s="5" t="s">
+      <c r="K4" s="1"/>
+      <c r="N4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1187,26 +1218,32 @@
       <c r="F5" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="N5" s="10" t="s">
+      <c r="O5" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1225,21 +1262,27 @@
       <c r="F6" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
@@ -1256,25 +1299,31 @@
         <v>1</v>
       </c>
       <c r="F7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="N7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1291,19 +1340,25 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1322,17 +1377,23 @@
       <c r="F9" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="N9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O9" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -1351,17 +1412,23 @@
       <c r="F10" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O10" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1380,20 +1447,26 @@
       <c r="F11" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="N11" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="M11" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O11" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>86</v>
       </c>
@@ -1412,17 +1485,23 @@
       <c r="F12" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="M12" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O12" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -1441,23 +1520,29 @@
       <c r="F13" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="7" t="s">
+      <c r="O13" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1476,20 +1561,26 @@
       <c r="F14" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="N14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O14" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
@@ -1508,23 +1599,29 @@
       <c r="F15" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="N15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M15" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N15" s="7" t="s">
+      <c r="O15" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P15" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
@@ -1543,17 +1640,23 @@
       <c r="F16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="N16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O16" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>158</v>
       </c>
@@ -1572,17 +1675,23 @@
       <c r="F17" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="N17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M17" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O17" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>161</v>
       </c>
@@ -1601,17 +1710,23 @@
       <c r="F18" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="N18" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="M18" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O18" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -1630,26 +1745,32 @@
       <c r="F19" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="N19" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M19" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N19" s="7" t="s">
+      <c r="O19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="O19" s="5" t="s">
+      <c r="Q19" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>147</v>
       </c>
@@ -1668,23 +1789,29 @@
       <c r="F20" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="N20" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="M20" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N20" s="7" t="s">
+      <c r="O20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>149</v>
       </c>
@@ -1703,19 +1830,25 @@
       <c r="F21" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="N21" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="M21" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" s="7" t="s">
+      <c r="O21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P21" s="7" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1728,10 +1861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1740,19 +1873,19 @@
     <col min="2" max="2" width="66.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="5"/>
-    <col min="10" max="10" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="44.5" style="7" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="5"/>
+    <col min="5" max="7" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="5"/>
+    <col min="12" max="12" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="44.5" style="7" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1769,37 +1902,43 @@
         <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1816,19 +1955,25 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O2" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>139</v>
       </c>
@@ -1847,17 +1992,23 @@
       <c r="F3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="M3" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>136</v>
       </c>
@@ -1874,19 +2025,25 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="M4" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O4" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>133</v>
       </c>
@@ -1903,26 +2060,32 @@
         <v>1</v>
       </c>
       <c r="F5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="M5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>130</v>
       </c>
@@ -1941,18 +2104,24 @@
       <c r="F6" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="M6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>128</v>
       </c>
@@ -1971,17 +2140,23 @@
       <c r="F7" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="N7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="M7" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O7" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>125</v>
       </c>
@@ -1998,22 +2173,28 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="M8" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>122</v>
       </c>
@@ -2032,20 +2213,26 @@
       <c r="F9" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="N9" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="M9" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O9" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>119</v>
       </c>
@@ -2064,17 +2251,23 @@
       <c r="F10" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="M10" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O10" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>116</v>
       </c>
@@ -2093,17 +2286,23 @@
       <c r="F11" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="N11" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="M11" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O11" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>108</v>
       </c>
@@ -2122,17 +2321,23 @@
       <c r="F12" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="M12" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O12" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>105</v>
       </c>
@@ -2151,17 +2356,23 @@
       <c r="F13" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="M13" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O13" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>113</v>
       </c>
@@ -2180,17 +2391,23 @@
       <c r="F14" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="N14" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O14" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>110</v>
       </c>
@@ -2209,17 +2426,23 @@
       <c r="F15" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="N15" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="M15" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O15" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>102</v>
       </c>
@@ -2238,18 +2461,24 @@
       <c r="F16" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="N16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="M16" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M18" s="10"/>
+      <c r="O16" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O18" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:C16" xr:uid="{692A23DE-1971-9644-BCB5-0858E868D84D}"/>
@@ -2260,10 +2489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
-  <dimension ref="A1:O1000"/>
+  <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2272,19 +2501,19 @@
     <col min="2" max="2" width="88.1640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.5" style="7" customWidth="1"/>
-    <col min="9" max="9" width="35.83203125" style="7" customWidth="1"/>
-    <col min="10" max="11" width="10.5" style="7" customWidth="1"/>
-    <col min="12" max="12" width="44.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="44.5" style="7" customWidth="1"/>
-    <col min="15" max="15" width="18.5" style="7" customWidth="1"/>
-    <col min="16" max="30" width="10.5" style="7" customWidth="1"/>
-    <col min="31" max="16384" width="11.1640625" style="7"/>
+    <col min="5" max="7" width="21.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5" style="7" customWidth="1"/>
+    <col min="11" max="11" width="35.83203125" style="7" customWidth="1"/>
+    <col min="12" max="13" width="10.5" style="7" customWidth="1"/>
+    <col min="14" max="14" width="44.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="44.5" style="7" customWidth="1"/>
+    <col min="17" max="17" width="18.5" style="7" customWidth="1"/>
+    <col min="18" max="32" width="10.5" style="7" customWidth="1"/>
+    <col min="33" max="16384" width="11.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2301,37 +2530,43 @@
         <v>153</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -2348,19 +2583,25 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>98</v>
       </c>
@@ -2377,25 +2618,31 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>95</v>
       </c>
@@ -2412,19 +2659,25 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="O4" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>92</v>
       </c>
@@ -2440,21 +2693,27 @@
       <c r="E5" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="M5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>89</v>
       </c>
@@ -2470,21 +2729,27 @@
       <c r="E6" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="N6" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="M6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>86</v>
       </c>
@@ -2503,20 +2768,26 @@
       <c r="F7" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="M7" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O7" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>82</v>
       </c>
@@ -2533,28 +2804,34 @@
         <v>1</v>
       </c>
       <c r="F8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="M8" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N8" s="7" t="s">
+      <c r="O8" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="Q8" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>79</v>
       </c>
@@ -2573,17 +2850,23 @@
       <c r="F9" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="M9" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O9" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>76</v>
       </c>
@@ -2602,17 +2885,23 @@
       <c r="F10" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="N10" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="M10" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O10" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>74</v>
       </c>
@@ -2629,29 +2918,35 @@
         <v>1</v>
       </c>
       <c r="F11" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="N11" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M11" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" s="7" t="s">
+      <c r="O11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P11" s="7" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3644,10 +3939,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4CB50-F135-6F43-A6BC-AC27D4D7EACE}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="B1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3656,18 +3951,18 @@
     <col min="2" max="2" width="68.1640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="5"/>
-    <col min="9" max="9" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="5"/>
-    <col min="12" max="12" width="23.6640625" style="5" customWidth="1"/>
-    <col min="13" max="14" width="44.5" style="7" customWidth="1"/>
-    <col min="15" max="15" width="140.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="5"/>
+    <col min="5" max="7" width="22.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" style="5"/>
+    <col min="11" max="11" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="5"/>
+    <col min="14" max="14" width="23.6640625" style="5" customWidth="1"/>
+    <col min="15" max="16" width="44.5" style="7" customWidth="1"/>
+    <col min="17" max="17" width="140.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3684,37 +3979,43 @@
         <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -3731,19 +4032,25 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O2" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>70</v>
       </c>
@@ -3760,18 +4067,24 @@
       <c r="F3" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="L3" s="5" t="s">
+      <c r="K3" s="1"/>
+      <c r="N3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>68</v>
       </c>
@@ -3787,23 +4100,29 @@
       <c r="F4" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>65</v>
       </c>
@@ -3819,34 +4138,44 @@
       <c r="F5" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="M5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E6" s="10"/>
-      <c r="F6" s="7"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="7"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>

</xml_diff>

<commit_message>
update to schema 1.5
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.5.xlsx
+++ b/schema_definitions/template_schema_v1.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Desktop/__FUNNY__/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhayhurst/Documents/projects/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DBB7ED-4C03-0E4E-97C2-05BECA83FC89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D605816-9C02-F74A-B51B-1DB9D516CF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="36860" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="-10640" yWindow="-18440" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="184">
   <si>
     <t>NAME</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>MANDATORY-GCST</t>
+  </si>
+  <si>
+    <t>Afghanistan|Albania|Algeria|American Samoa|Andorra|Angola|Anguilla|Antigua and Barbuda|Argentina|Armenia|Australia|Austria|Azerbaijan|Bahamas|Bahrain|Bangladesh|Barbados|Belarus|Belgium|Belize|Benin|Bermuda|Bhutan|Bolivia|Bosnia and Herzegovina|Botswana|Brazil|British Virgin Islands|Brunei Darussalam|Bulgaria|Burkina Faso|Burundi|Cambodia|Cameroon|Canada|Cape Verde|Cayman Islands|Central African Republic|Chad|Channel Islands|Chile|China|China, Hong Kong SAR|China, Macao SAR|Colombia|Comoros|Congo|Cook Islands|Costa Rica|Croatia|Cuba|Cyprus|Cyprus|Czech Republic|Côte d’Ivoire|Democratic People’s Republic of Korea|Democratic Republic of the Congo|Denmark|Djibouti|Dominica|Dominican Republic|Ecuador|Egypt|El Salvador|Equatorial Guinea|Eritrea|Estonia|Ethiopia|Faeroe Islands|Falkland Islands (Malvinas)|Fiji|Finland|France|French Guiana|French Polynesia|Gabon|Gambia|Georgia|Germany|Ghana|Gibraltar|Greece|Greenland|Grenada|Guadeloupe|Guam|Guatemala|Guinea|Guinea-Bissau|Guyana|Haiti|Holy See|Honduras|Hungary|Iceland|India|Indonesia|Iran (Islamic Republic of)|Iraq|Isle of Man|Israel|Italy|Jamaica|Japan|Jordan|Kazakhstan|Kenya|Kiribati|Kuwait|Kyrgyzstan|Lao People’s Democratic Republic|Latvia|Lebanon|Lesotho|Liberia|Libyan Arab Jamahiriya|Liechtenstein|Lithuania|Luxembourg|Madagascar|Malawi|Malaysia|Maldives|Mali|Malta|Marshall Islands|Martinique|Mauretania|Mauritius|Mayotte|Mexico|Micronesia (Federated States of)|Monaco|Mongolia|Montenegro|Montserrat|Morocco|Mozambique|Myanmar|NR|Namibia|Nauru|Nepal|Netherlands|Netherlands Antilles|New Caledonia|New Zealand|Nicaragua|Niger|Nigeria|Niue|Norfolk Island|Norway|Occupied Palestinian Territory|Oman|Pakistan|Palau|Panama|Papua New Guinea|Paraguay|Peru|Philippines|Pitcairn|Poland|Portugal|Puerto Rico|Qatar|Republic of Ireland|Republic of Korea|Republic of Moldova|Romania|Russian Federation|Rwanda|Réunion|Saint Kitts and Nevis|Saint Lucia|Saint Vincent and the Grenadines|Saint-Pierre-et-Miquelon|Samoa|San Marino|Saudi Arabia|Senegal|Serbia|Seychelles|Sierra Leone|Singapore|Slovakia|Slovenia|Solomon Islands|Somalia|South Africa|Spain|Sri Lanka|St. Helena|Sudan|Suriname|Swaziland|Sweden|Switzerland|São Tomé and Príncipe|Taiwan|Tajikistan|Thailand|The former Yugoslav Republic of Macedonia|Timor-Leste|Togo|Tokelau|Tonga|Trinidad and Tobago|Tunisia|Turkey|Turkmenistan|Turks and Caicos Islands|Tuvalu|U.K.|U.S.|U.S. Virgin Islands|Uganda|Ukraine|United Arab Emirates|United Republic of Tanzania|Uruguay|Uzbekistan|Vanuatu|Venezuela|Viet Nam|Wallis and Futuna Islands|Western Sahara|Yemen|Zambia|Zimbabwe</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -2491,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2940,6 +2943,9 @@
       </c>
       <c r="P11" s="7" t="s">
         <v>171</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>